<commit_message>
Maxxcard - alteracoes no esforco
</commit_message>
<xml_diff>
--- a/documentacao/maxxcard/maxxcard_esforco.xlsx
+++ b/documentacao/maxxcard/maxxcard_esforco.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
   <si>
     <t xml:space="preserve">Projeto</t>
   </si>
@@ -100,21 +100,48 @@
     <t xml:space="preserve">Incluir parâmetro para Limite Mensal</t>
   </si>
   <si>
-    <t xml:space="preserve">2.Faturamento CAP Estabelecimentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.Cadastro de Estabelecimento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP por fechamento</t>
+    <t xml:space="preserve">1.6. Homologação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.CAP Estabelecimentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.Cadastro da Administradora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definir ciclos de fechamento gerais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incluir interface de configuração de ciclos de fechamento gerais (padrão)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2.Cadastro de Estabelecimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definir ciclos de fechamentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incluir interface de configuração de ciclos de fechamento específicos por estabelecimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3. Faturamento</t>
   </si>
   <si>
     <t xml:space="preserve">Faturamento de Contas</t>
   </si>
   <si>
+    <t xml:space="preserve">Faturamento das Contas Estab por ciclo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Geração arquivo pagamento BRADESCO</t>
   </si>
   <si>
+    <t xml:space="preserve">Geração dos arquivos de pagamento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4. Homologação</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.Faturamento CAR Conveniados (modelo crédito)</t>
   </si>
   <si>
@@ -136,7 +163,7 @@
     <t xml:space="preserve">Definir prazo para pagamento fatura</t>
   </si>
   <si>
-    <t xml:space="preserve">Incluir parâmetro para definição </t>
+    <t xml:space="preserve">Incluir parâmetro para definição da data de vencimento da fatura</t>
   </si>
   <si>
     <t xml:space="preserve">Definir juros pró-rata por atraso</t>
@@ -169,21 +196,39 @@
     <t xml:space="preserve">CAR por fechamento</t>
   </si>
   <si>
+    <t xml:space="preserve">Agendamento de lançamentos financeiros do CAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.3. Faturamento </t>
   </si>
   <si>
     <t xml:space="preserve">Faturamento Contas </t>
   </si>
   <si>
+    <t xml:space="preserve">Faturamento de Contas em situação normal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Faturamento Contas em Atraso</t>
   </si>
   <si>
+    <t xml:space="preserve">Faturamento de Contas em situação de atraso</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gerar boletos ITAÚ</t>
   </si>
   <si>
+    <t xml:space="preserve">Geração de Boletos </t>
+  </si>
+  <si>
     <t xml:space="preserve">Gerar arquivo Registro Cobrança ITAÚ</t>
   </si>
   <si>
+    <t xml:space="preserve">Geração do Arquivo cobrança</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processamento Arquivo Retorno Cobrança</t>
+  </si>
+  <si>
     <t xml:space="preserve">4. Liquidação de Faturas</t>
   </si>
   <si>
@@ -199,7 +244,7 @@
     <t xml:space="preserve">Processar atualização de contas</t>
   </si>
   <si>
-    <t xml:space="preserve">Processamento de atualização os saldos de portadores após o faturamento para eventuais </t>
+    <t xml:space="preserve">Processamento de atualização os saldos de portadores após o faturamento</t>
   </si>
   <si>
     <t xml:space="preserve">6.Controle de Adimplência/Inadimplência</t>
@@ -208,6 +253,9 @@
     <t xml:space="preserve">Processar bloqueio/desbloqueio de contas</t>
   </si>
   <si>
+    <t xml:space="preserve">Homologação</t>
+  </si>
+  <si>
     <t xml:space="preserve">7.Produtos/Serviços</t>
   </si>
   <si>
@@ -221,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve">Refactoring Transação de Combustível</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adaptação das regras para contemplar cartão associado a veiculo</t>
   </si>
   <si>
     <t xml:space="preserve">Refactoring Transação de Serviços</t>
@@ -376,18 +427,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.86734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="94.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.86734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,367 +470,356 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>10</v>
-      </c>
+      <c r="A8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B13" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
+      <c r="A19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>27</v>
+      <c r="A20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" s="3" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>38</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" s="3" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>40</v>
+      <c r="A30" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
+      <c r="B41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C41" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="B45" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="B46" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
-        <v>54</v>
+      <c r="B47" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="5" t="n">
+      <c r="B50" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
+      <c r="C53" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="0" t="n">
+    </row>
+    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="C51" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+      <c r="C56" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <v>21</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,45 +827,174 @@
         <v>64</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <v>21</v>
+      <c r="A60" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>21</v>
+      <c r="A62" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" s="0" t="n">
-        <v>21</v>
-      </c>
+      <c r="A63" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="7" t="n">
-        <f aca="false">SUM(B6:B63)</f>
-        <v>612</v>
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" s="7" t="n">
+        <f aca="false">SUM(B7:B81)</f>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>